<commit_message>
enabled add parcel feature
</commit_message>
<xml_diff>
--- a/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
+++ b/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p57448\Downloads\CargoUIAutomation_Refactored\CargoUIAutomation\CargoUIAutomation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IdeaProjects\Cargo\CargoUIAutomationNew\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AA1422-110E-4AB2-B512-9CBD247EA740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8ACFFBD-16CD-4A9E-A8BE-BFDB46140611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="343">
   <si>
     <t>CargoUsernameLogin</t>
   </si>
@@ -705,21 +705,9 @@
     <t>input#gestationDestCode</t>
   </si>
   <si>
-    <t>input#gequantity-1</t>
-  </si>
-  <si>
     <t>input#gestationSourceCode</t>
   </si>
   <si>
-    <t>input#gelength-1</t>
-  </si>
-  <si>
-    <t>input#gewidth-1</t>
-  </si>
-  <si>
-    <t>input#geheight-1</t>
-  </si>
-  <si>
     <t>div#dc-tab-content156-6406 &gt; form &gt; div:nth-child(7) &gt; a</t>
   </si>
   <si>
@@ -1023,9 +1011,6 @@
     <t>//span[@id='awbNumber']</t>
   </si>
   <si>
-    <t>select#geunit-1 option</t>
-  </si>
-  <si>
     <t>select#getotalWeightUnit option</t>
   </si>
   <si>
@@ -1036,6 +1021,39 @@
   </si>
   <si>
     <t>#mainContent &gt; dc-flight-search-results &gt; div &gt; div.sticky-container &gt; div:nth-child(2) &gt; div &gt; div &gt; div &gt; div:nth-child(1) &gt; div:nth-child(3)</t>
+  </si>
+  <si>
+    <t>gbParcelAddParcel</t>
+  </si>
+  <si>
+    <t>Add Parcel</t>
+  </si>
+  <si>
+    <t>input#gequantity-%s</t>
+  </si>
+  <si>
+    <t>input#gelength-%s</t>
+  </si>
+  <si>
+    <t>input#gewidth-%s</t>
+  </si>
+  <si>
+    <t>input#geheight-%s</t>
+  </si>
+  <si>
+    <t>select#geunit-%s option</t>
+  </si>
+  <si>
+    <t>gbParcelUnitSelect</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-content']</t>
+  </si>
+  <si>
+    <t>gbParcelUnitSelectOk</t>
+  </si>
+  <si>
+    <t>//button[text()='OK']</t>
   </si>
 </sst>
 </file>
@@ -1429,21 +1447,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486E0D93-E580-4D4E-91BE-77049C6FF4F1}">
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="56.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="56.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="73.5" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.75" style="1"/>
+    <col min="4" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5">
+    <row r="1" spans="1:3" ht="16.8">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5">
+    <row r="2" spans="1:3" ht="16.8">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5">
+    <row r="3" spans="1:3" ht="16.8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1467,7 +1485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5">
+    <row r="4" spans="1:3" ht="16.8">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5">
+    <row r="5" spans="1:3" ht="16.8">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5">
+    <row r="6" spans="1:3" ht="16.8">
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
@@ -1491,7 +1509,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5">
+    <row r="7" spans="1:3" ht="16.8">
       <c r="A7" s="2" t="s">
         <v>172</v>
       </c>
@@ -1499,7 +1517,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5">
+    <row r="8" spans="1:3" ht="16.8">
       <c r="A8" s="2" t="s">
         <v>174</v>
       </c>
@@ -1507,7 +1525,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5">
+    <row r="9" spans="1:3" ht="16.8">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1515,7 +1533,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5">
+    <row r="10" spans="1:3" ht="16.8">
       <c r="A10" s="2" t="s">
         <v>179</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5">
+    <row r="11" spans="1:3" ht="16.8">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1535,7 +1553,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="16.5">
+    <row r="12" spans="1:3" ht="16.8">
       <c r="A12" s="2" t="s">
         <v>180</v>
       </c>
@@ -1544,7 +1562,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="16.5">
+    <row r="13" spans="1:3" ht="16.8">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1570,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5">
+    <row r="14" spans="1:3" ht="16.8">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1560,7 +1578,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5">
+    <row r="15" spans="1:3" ht="16.8">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1568,7 +1586,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5">
+    <row r="16" spans="1:3" ht="16.8">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1576,7 +1594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.5">
+    <row r="17" spans="1:2" ht="16.8">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1584,7 +1602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.5">
+    <row r="18" spans="1:2" ht="16.8">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1592,7 +1610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5">
+    <row r="19" spans="1:2" ht="16.8">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1600,7 +1618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.5">
+    <row r="20" spans="1:2" ht="16.8">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1608,7 +1626,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5">
+    <row r="21" spans="1:2" ht="16.8">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1616,7 +1634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5">
+    <row r="22" spans="1:2" ht="16.8">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1624,7 +1642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5">
+    <row r="23" spans="1:2" ht="16.8">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1650,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.5">
+    <row r="24" spans="1:2" ht="16.8">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1640,7 +1658,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.5">
+    <row r="25" spans="1:2" ht="16.8">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1648,7 +1666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.5">
+    <row r="26" spans="1:2" ht="16.8">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5">
+    <row r="27" spans="1:2" ht="16.8">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1664,7 +1682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.5">
+    <row r="28" spans="1:2" ht="16.8">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1672,7 +1690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16.5">
+    <row r="29" spans="1:2" ht="16.8">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1680,7 +1698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.5">
+    <row r="30" spans="1:2" ht="16.8">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1688,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.5">
+    <row r="31" spans="1:2" ht="16.8">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1696,7 +1714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.5">
+    <row r="32" spans="1:2" ht="16.8">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -1704,7 +1722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.5">
+    <row r="33" spans="1:2" ht="16.8">
       <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
@@ -1712,7 +1730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16.5">
+    <row r="34" spans="1:2" ht="16.8">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -1720,7 +1738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.5">
+    <row r="35" spans="1:2" ht="16.8">
       <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
@@ -1728,7 +1746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16.5">
+    <row r="36" spans="1:2" ht="16.8">
       <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
@@ -1736,7 +1754,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.5">
+    <row r="37" spans="1:2" ht="16.8">
       <c r="A37" s="2" t="s">
         <v>56</v>
       </c>
@@ -1744,7 +1762,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.5">
+    <row r="38" spans="1:2" ht="16.8">
       <c r="A38" s="2" t="s">
         <v>58</v>
       </c>
@@ -1752,7 +1770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.5">
+    <row r="39" spans="1:2" ht="16.8">
       <c r="A39" s="2" t="s">
         <v>60</v>
       </c>
@@ -1760,7 +1778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.5">
+    <row r="40" spans="1:2" ht="16.8">
       <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
@@ -1768,7 +1786,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16.5">
+    <row r="41" spans="1:2" ht="16.8">
       <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
@@ -1776,7 +1794,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.5">
+    <row r="42" spans="1:2" ht="16.8">
       <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
@@ -1784,7 +1802,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.5">
+    <row r="43" spans="1:2" ht="16.8">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16.5">
+    <row r="44" spans="1:2" ht="16.8">
       <c r="A44" s="2" t="s">
         <v>70</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16.5">
+    <row r="45" spans="1:2" ht="16.8">
       <c r="A45" s="2" t="s">
         <v>72</v>
       </c>
@@ -1808,7 +1826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16.5">
+    <row r="46" spans="1:2" ht="16.8">
       <c r="A46" s="2" t="s">
         <v>74</v>
       </c>
@@ -1816,7 +1834,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16.5">
+    <row r="47" spans="1:2" ht="16.8">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
@@ -1824,7 +1842,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.5">
+    <row r="48" spans="1:2" ht="16.8">
       <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
@@ -1832,7 +1850,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.5">
+    <row r="49" spans="1:2" ht="16.8">
       <c r="A49" s="2" t="s">
         <v>80</v>
       </c>
@@ -1840,7 +1858,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.5">
+    <row r="50" spans="1:2" ht="16.8">
       <c r="A50" s="2" t="s">
         <v>82</v>
       </c>
@@ -1848,7 +1866,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16.5">
+    <row r="51" spans="1:2" ht="16.8">
       <c r="A51" s="2" t="s">
         <v>84</v>
       </c>
@@ -1856,7 +1874,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.5">
+    <row r="52" spans="1:2" ht="16.8">
       <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
@@ -1864,7 +1882,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16.5">
+    <row r="53" spans="1:2" ht="16.8">
       <c r="A53" s="2" t="s">
         <v>88</v>
       </c>
@@ -1872,7 +1890,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16.5">
+    <row r="54" spans="1:2" ht="16.8">
       <c r="A54" s="2" t="s">
         <v>90</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.5">
+    <row r="55" spans="1:2" ht="16.8">
       <c r="A55" s="2" t="s">
         <v>92</v>
       </c>
@@ -1888,7 +1906,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.5">
+    <row r="56" spans="1:2" ht="16.8">
       <c r="A56" s="2" t="s">
         <v>94</v>
       </c>
@@ -1896,7 +1914,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16.5">
+    <row r="57" spans="1:2" ht="16.8">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -1904,7 +1922,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16.5">
+    <row r="58" spans="1:2" ht="16.8">
       <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
@@ -1912,7 +1930,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.5">
+    <row r="59" spans="1:2" ht="16.8">
       <c r="A59" s="2" t="s">
         <v>100</v>
       </c>
@@ -1920,7 +1938,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.5">
+    <row r="60" spans="1:2" ht="16.8">
       <c r="A60" s="2" t="s">
         <v>102</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.5">
+    <row r="61" spans="1:2" ht="16.8">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -1936,7 +1954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.5">
+    <row r="62" spans="1:2" ht="16.8">
       <c r="A62" s="2" t="s">
         <v>106</v>
       </c>
@@ -1944,7 +1962,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.5">
+    <row r="63" spans="1:2" ht="16.8">
       <c r="A63" s="2" t="s">
         <v>108</v>
       </c>
@@ -1952,7 +1970,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.5">
+    <row r="64" spans="1:2" ht="16.8">
       <c r="A64" s="2" t="s">
         <v>110</v>
       </c>
@@ -1960,7 +1978,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16.5">
+    <row r="65" spans="1:2" ht="16.8">
       <c r="A65" s="2" t="s">
         <v>112</v>
       </c>
@@ -1968,7 +1986,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16.5">
+    <row r="66" spans="1:2" ht="16.8">
       <c r="A66" s="2" t="s">
         <v>114</v>
       </c>
@@ -1976,7 +1994,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.5">
+    <row r="67" spans="1:2" ht="16.8">
       <c r="A67" s="2" t="s">
         <v>116</v>
       </c>
@@ -1984,7 +2002,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16.5">
+    <row r="68" spans="1:2" ht="16.8">
       <c r="A68" s="2" t="s">
         <v>118</v>
       </c>
@@ -1992,7 +2010,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16.5">
+    <row r="69" spans="1:2" ht="16.8">
       <c r="A69" s="2" t="s">
         <v>120</v>
       </c>
@@ -2000,7 +2018,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16.5">
+    <row r="70" spans="1:2" ht="16.8">
       <c r="A70" s="2" t="s">
         <v>122</v>
       </c>
@@ -2008,7 +2026,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="16.5">
+    <row r="71" spans="1:2" ht="16.8">
       <c r="A71" s="2" t="s">
         <v>124</v>
       </c>
@@ -2016,7 +2034,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.5">
+    <row r="72" spans="1:2" ht="16.8">
       <c r="A72" s="2" t="s">
         <v>126</v>
       </c>
@@ -2024,7 +2042,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.5">
+    <row r="73" spans="1:2" ht="16.8">
       <c r="A73" s="2" t="s">
         <v>128</v>
       </c>
@@ -2032,7 +2050,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16.5">
+    <row r="74" spans="1:2" ht="16.8">
       <c r="A74" s="2" t="s">
         <v>129</v>
       </c>
@@ -2040,7 +2058,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16.5">
+    <row r="75" spans="1:2" ht="16.8">
       <c r="A75" s="2" t="s">
         <v>131</v>
       </c>
@@ -2048,7 +2066,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.5">
+    <row r="76" spans="1:2" ht="16.8">
       <c r="A76" s="2" t="s">
         <v>133</v>
       </c>
@@ -2056,7 +2074,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16.5">
+    <row r="77" spans="1:2" ht="16.8">
       <c r="A77" s="2" t="s">
         <v>135</v>
       </c>
@@ -2064,7 +2082,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16.5">
+    <row r="78" spans="1:2" ht="16.8">
       <c r="A78" s="2" t="s">
         <v>137</v>
       </c>
@@ -2072,7 +2090,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.5">
+    <row r="79" spans="1:2" ht="16.8">
       <c r="A79" s="2" t="s">
         <v>139</v>
       </c>
@@ -2080,7 +2098,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16.5">
+    <row r="80" spans="1:2" ht="16.8">
       <c r="A80" s="2" t="s">
         <v>141</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16.5">
+    <row r="81" spans="1:2" ht="16.8">
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
@@ -2096,7 +2114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16.5">
+    <row r="82" spans="1:2" ht="16.8">
       <c r="A82" s="2" t="s">
         <v>143</v>
       </c>
@@ -2104,7 +2122,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16.5">
+    <row r="83" spans="1:2" ht="16.8">
       <c r="A83" s="2" t="s">
         <v>145</v>
       </c>
@@ -2112,7 +2130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16.5">
+    <row r="84" spans="1:2" ht="16.8">
       <c r="A84" s="2" t="s">
         <v>147</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16.5">
+    <row r="85" spans="1:2" ht="16.8">
       <c r="A85" s="2" t="s">
         <v>149</v>
       </c>
@@ -2128,7 +2146,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16.5">
+    <row r="86" spans="1:2" ht="16.8">
       <c r="A86" s="2" t="s">
         <v>151</v>
       </c>
@@ -2136,7 +2154,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16.5">
+    <row r="87" spans="1:2" ht="16.8">
       <c r="A87" s="2" t="s">
         <v>153</v>
       </c>
@@ -2144,7 +2162,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16.5">
+    <row r="88" spans="1:2" ht="16.8">
       <c r="A88" s="2" t="s">
         <v>155</v>
       </c>
@@ -2152,7 +2170,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16.5">
+    <row r="89" spans="1:2" ht="16.8">
       <c r="A89" s="2" t="s">
         <v>157</v>
       </c>
@@ -2160,7 +2178,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16.5">
+    <row r="90" spans="1:2" ht="16.8">
       <c r="A90" s="2" t="s">
         <v>159</v>
       </c>
@@ -2168,7 +2186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16.5">
+    <row r="91" spans="1:2" ht="16.8">
       <c r="A91" s="2" t="s">
         <v>160</v>
       </c>
@@ -2176,7 +2194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16.5">
+    <row r="92" spans="1:2" ht="16.8">
       <c r="A92" s="2" t="s">
         <v>161</v>
       </c>
@@ -2184,7 +2202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16.5">
+    <row r="93" spans="1:2" ht="16.8">
       <c r="A93" s="2" t="s">
         <v>162</v>
       </c>
@@ -2192,7 +2210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16.5">
+    <row r="94" spans="1:2" ht="16.8">
       <c r="A94" s="2" t="s">
         <v>163</v>
       </c>
@@ -2200,7 +2218,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16.5">
+    <row r="95" spans="1:2" ht="16.8">
       <c r="A95" s="2" t="s">
         <v>165</v>
       </c>
@@ -2208,7 +2226,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16.5">
+    <row r="96" spans="1:2" ht="16.8">
       <c r="A96" s="2" t="s">
         <v>167</v>
       </c>
@@ -2293,7 +2311,7 @@
         <v>203</v>
       </c>
       <c r="B106" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2306,50 +2324,50 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2357,7 +2375,7 @@
         <v>205</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2365,23 +2383,23 @@
         <v>206</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2397,7 +2415,7 @@
         <v>208</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>226</v>
+        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2405,7 +2423,7 @@
         <v>209</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>228</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2413,7 +2431,7 @@
         <v>210</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>229</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2421,7 +2439,7 @@
         <v>211</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>230</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2429,92 +2447,92 @@
         <v>212</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
-        <v>213</v>
+        <v>339</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>231</v>
+        <v>340</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="1" t="s">
-        <v>214</v>
+        <v>341</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1" t="s">
-        <v>215</v>
+        <v>332</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>240</v>
+        <v>333</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>333</v>
+        <v>227</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>236</v>
+        <v>328</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>233</v>
@@ -2522,338 +2540,362 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>305</v>
+        <v>221</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>306</v>
+        <v>234</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>307</v>
+        <v>222</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>308</v>
+        <v>235</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>309</v>
+        <v>223</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>310</v>
+        <v>229</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>334</v>
+        <v>301</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1" t="s">
-        <v>245</v>
+        <v>324</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>246</v>
+        <v>325</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="1" t="s">
-        <v>260</v>
+        <v>326</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="1" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>300</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>53</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>285</v>
+        <v>53</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor and some minor changes
</commit_message>
<xml_diff>
--- a/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
+++ b/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IdeaProjects\Cargo\CargoUIAutomationNew\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5B2D04-CB27-4EA0-8A86-11EF545C5E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2299BA6-D277-4B6D-B73A-D922A4A13943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16797" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16799" uniqueCount="400">
   <si>
     <t>CargoUsernameLogin</t>
   </si>
@@ -1212,13 +1212,19 @@
     <t>select[id='phtotalWeightUnit']</t>
   </si>
   <si>
-    <t>gbPharmaSelectTotalWeightType</t>
-  </si>
-  <si>
     <t>select[id='phpharmaType-%s']</t>
   </si>
   <si>
     <t>input[id='getotalWeight']</t>
+  </si>
+  <si>
+    <t>gbPharmaSelectTotalWeightUnit</t>
+  </si>
+  <si>
+    <t>gbPharmaFindFlights</t>
+  </si>
+  <si>
+    <t>div[class='dc-clear'] + button[type='submit']</t>
   </si>
 </sst>
 </file>
@@ -1612,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486E0D93-E580-4D4E-91BE-77049C6FF4F1}">
-  <dimension ref="A1:XFD207"/>
+  <dimension ref="A1:XFD208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
@@ -2660,7 +2666,7 @@
         <v>215</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -52262,7 +52268,7 @@
         <v>353</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="187" spans="1:16384">
@@ -52387,7 +52393,7 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>394</v>
@@ -52431,6 +52437,14 @@
       </c>
       <c r="B207" s="1" t="s">
         <v>377</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed couple of bugs
</commit_message>
<xml_diff>
--- a/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
+++ b/CargoUIAutomationNew/src/test/resources/XpathTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IdeaProjects\Cargo\CargoUIAutomationNew\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2299BA6-D277-4B6D-B73A-D922A4A13943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F515C23-EB75-43AC-BF0F-A096524B5F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73F83708-58D9-CD41-B3DD-01428282C24F}"/>
   </bookViews>
@@ -1200,9 +1200,6 @@
     <t>gbPharmaUnit</t>
   </si>
   <si>
-    <t>input[id='phunit-%s']</t>
-  </si>
-  <si>
     <t>gbPharmaAddItem</t>
   </si>
   <si>
@@ -1225,6 +1222,9 @@
   </si>
   <si>
     <t>div[class='dc-clear'] + button[type='submit']</t>
+  </si>
+  <si>
+    <t>select[id='phunit-%s']</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1621,7 @@
   <dimension ref="A1:XFD208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A208" sqref="A208"/>
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
@@ -2666,7 +2666,7 @@
         <v>215</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -52268,7 +52268,7 @@
         <v>353</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="187" spans="1:16384">
@@ -52364,15 +52364,15 @@
         <v>390</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -52393,10 +52393,10 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -52441,10 +52441,10 @@
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>